<commit_message>
Completed XLSX with benchmark results
</commit_message>
<xml_diff>
--- a/04/Exercise_1/results/benchmark.xlsx
+++ b/04/Exercise_1/results/benchmark.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fabia\Documents\ps_parprog_2024_shared\04\Exercise_1\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{72BEB4E0-4B6A-4145-BE10-A2D46267F41A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A53AF8E1-400B-4C3C-8031-714FFB778A45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9B99442A-7CAB-4A04-92C1-B2DB71FCC5D8}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9B99442A-7CAB-4A04-92C1-B2DB71FCC5D8}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -44,16 +44,16 @@
     <t>Implementation</t>
   </si>
   <si>
-    <t>Threads</t>
+    <t>Pthread</t>
   </si>
   <si>
-    <t>Critical [omp]</t>
+    <t>OMP (Atomic)</t>
   </si>
   <si>
-    <t>Atomic [omp]</t>
+    <t>OMP (Reduction)</t>
   </si>
   <si>
-    <t>Reduction [omp]</t>
+    <t>OMP (Critical)</t>
   </si>
 </sst>
 </file>
@@ -205,7 +205,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Threads</c:v>
+                  <c:v>Pthread</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -265,19 +265,19 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>10.878</c:v>
+                  <c:v>10.898999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.5</c:v>
+                  <c:v>5.4550000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.754</c:v>
+                  <c:v>2.7570000000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.903</c:v>
+                  <c:v>1.8939999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.96399999999999997</c:v>
+                  <c:v>0.96199999999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -286,6 +286,285 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-3A23-413F-8690-5ADB8E65A002}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>OMP (Critical)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$A$3:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$C$3:$C$7</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>16.411000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>43.594000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>119.46599999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>152.977</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>176.399</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3A23-413F-8690-5ADB8E65A002}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>OMP (Atomic)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$A$3:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$D$3:$D$7</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>14.037000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.287000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24.861000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25.667000000000002</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20.593</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-3A23-413F-8690-5ADB8E65A002}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>OMP (Reduction)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Tabelle1!$A$3:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>12</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Tabelle1!$E$3:$E$7</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>10.335000000000001</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.1559999999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.6160000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.8740000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.98799999999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-3A23-413F-8690-5ADB8E65A002}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -304,6 +583,8 @@
         <c:axId val="800876799"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="12"/>
+          <c:min val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -416,11 +697,14 @@
         <c:crossAx val="800873439"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="1"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="800873439"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="180"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -542,6 +826,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -1146,16 +1461,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>52386</xdr:rowOff>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>38099</xdr:rowOff>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1503,7 +1818,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="R20" sqref="R20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1532,13 +1847,13 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1546,7 +1861,16 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>10.878</v>
+        <v>10.898999999999999</v>
+      </c>
+      <c r="C3" s="1">
+        <v>16.411000000000001</v>
+      </c>
+      <c r="D3" s="1">
+        <v>14.037000000000001</v>
+      </c>
+      <c r="E3" s="1">
+        <v>10.335000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1554,7 +1878,16 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>5.5</v>
+        <v>5.4550000000000001</v>
+      </c>
+      <c r="C4" s="1">
+        <v>43.594000000000001</v>
+      </c>
+      <c r="D4" s="1">
+        <v>12.287000000000001</v>
+      </c>
+      <c r="E4" s="1">
+        <v>5.1559999999999997</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1562,7 +1895,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="1">
-        <v>2.754</v>
+        <v>2.7570000000000001</v>
+      </c>
+      <c r="C5" s="1">
+        <v>119.46599999999999</v>
+      </c>
+      <c r="D5" s="1">
+        <v>24.861000000000001</v>
+      </c>
+      <c r="E5" s="1">
+        <v>2.6160000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1570,7 +1912,16 @@
         <v>6</v>
       </c>
       <c r="B6" s="1">
-        <v>1.903</v>
+        <v>1.8939999999999999</v>
+      </c>
+      <c r="C6" s="1">
+        <v>152.977</v>
+      </c>
+      <c r="D6" s="1">
+        <v>25.667000000000002</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1.8740000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1578,7 +1929,16 @@
         <v>12</v>
       </c>
       <c r="B7" s="1">
-        <v>0.96399999999999997</v>
+        <v>0.96199999999999997</v>
+      </c>
+      <c r="C7" s="1">
+        <v>176.399</v>
+      </c>
+      <c r="D7" s="1">
+        <v>20.593</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.98799999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>